<commit_message>
manual, fnc, op need cleaning
</commit_message>
<xml_diff>
--- a/Redesign/IO/OUTPUT/608-Inventory-format-2024 Thymes-Seasonal Gift-Dept 37.xlsx
+++ b/Redesign/IO/OUTPUT/608-Inventory-format-2024 Thymes-Seasonal Gift-Dept 37.xlsx
@@ -518,7 +518,11 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>TH02710190100</t>
@@ -561,7 +565,11 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>TH05010190100</t>
@@ -604,7 +612,11 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>TH03515200500</t>
@@ -647,7 +659,11 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>TH03505206510</t>
@@ -690,7 +706,11 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>TH03515289400</t>
@@ -733,7 +753,11 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>TH03505279320</t>
@@ -776,7 +800,11 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
           <t>TH03505205600</t>
@@ -819,7 +847,11 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>TH04010190200</t>
@@ -862,7 +894,11 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>TH03515289200</t>

</xml_diff>